<commit_message>
Got 90% test accuracy
</commit_message>
<xml_diff>
--- a/Homework4/EE6770_HW4_Trial_Tracker.xlsx
+++ b/Homework4/EE6770_HW4_Trial_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyiin/Library/CloudStorage/Dropbox/Personal/Job2020/Kennesaw/Courses Fall 2024/EE6770/Homework/Homework_4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrin\Documents\GitHub\EE-6770-Application_Neural_Network\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0187215E-0D59-BF42-B18C-B5EC6984792B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A91EA-701C-4881-99EE-867DB18F68D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2280" windowWidth="27640" windowHeight="16940" xr2:uid="{B15C916A-5E8B-A149-80FA-6229EC8406AD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B15C916A-5E8B-A149-80FA-6229EC8406AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Trial #</t>
   </si>
@@ -116,13 +116,26 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>* 3-Layer NN
+* n1 = 8
+* n2 = 8</t>
+  </si>
+  <si>
+    <t>validation_split=0.25</t>
+  </si>
+  <si>
+    <t>* 3-Layer NN
+* n1 = 10
+* n2 = 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +201,12 @@
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -239,22 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -282,6 +286,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,342 +644,484 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECD881C-90B5-3E4A-8289-E7A06430E593}">
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" customWidth="1"/>
     <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.625" customWidth="1"/>
     <col min="11" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" customWidth="1"/>
+    <col min="13" max="14" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:17" ht="45.95" customHeight="1">
+      <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="2:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+    </row>
+    <row r="2" spans="2:17" ht="30.95" customHeight="1">
+      <c r="B2" s="4"/>
+      <c r="C2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="2:17" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="2:17" ht="47.1" customHeight="1">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:17" ht="54" customHeight="1">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="10">
         <v>256</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="10">
         <v>0.2</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="10">
         <v>10000</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="10">
         <v>0.26889999999999997</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="11">
         <v>0.88129999999999997</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="10">
         <v>0.72629999999999995</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="11">
         <v>0.745</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="10">
         <v>0.36959999999999998</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="13">
         <v>0.83799999999999997</v>
       </c>
-      <c r="Q4" s="17"/>
-    </row>
-    <row r="5" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="10">
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="2:17" ht="50.25" customHeight="1">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="10">
+        <v>256</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>10000</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0.35020000000000001</v>
+      </c>
+      <c r="P5" s="13">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="2:17" ht="56.25" customHeight="1">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="10">
+        <v>256</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J6" s="10">
+        <v>10000</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.85150000000000003</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0.1903</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0.59179999999999999</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="2:17" ht="49.5" customHeight="1">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="10">
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="10">
+        <v>512</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="10">
+        <v>10000</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.35439999999999999</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.82820000000000005</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0.24610000000000001</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0.3856</v>
+      </c>
+      <c r="P7" s="13">
+        <v>0.83</v>
+      </c>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="2:17" ht="42.75">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-    </row>
-    <row r="9" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10">
+        <v>256</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="10">
+        <v>10000</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.9073</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0.46489999999999998</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0.28410000000000002</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0.87</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="42.75">
+      <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-    </row>
-    <row r="10" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-    </row>
-    <row r="12" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-    </row>
-    <row r="13" spans="2:17" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="10">
+        <v>256</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="10">
+        <v>10000</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0.45319999999999999</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="O9" s="10">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="2:17" ht="24.95" customHeight="1">
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+    </row>
+    <row r="11" spans="2:17" ht="24.95" customHeight="1">
+      <c r="B11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="2:17" ht="24.95" customHeight="1">
+      <c r="B12" s="5"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" spans="2:17" ht="24.95" customHeight="1">
+      <c r="B13" s="5"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="2:17">
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -978,7 +1139,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17">
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -996,7 +1157,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17">
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1014,7 +1175,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17">
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1032,7 +1193,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17">
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1050,7 +1211,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17">
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1068,7 +1229,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17">
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1086,7 +1247,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17">
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1104,7 +1265,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1128,6 +1289,7 @@
     <mergeCell ref="K2:P2"/>
     <mergeCell ref="E2:J2"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added notes to tracker file
</commit_message>
<xml_diff>
--- a/Homework4/EE6770_HW4_Trial_Tracker.xlsx
+++ b/Homework4/EE6770_HW4_Trial_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrin\Documents\GitHub\EE-6770-Application_Neural_Network\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A91EA-701C-4881-99EE-867DB18F68D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC704E-37FF-455C-996B-35795B39830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B15C916A-5E8B-A149-80FA-6229EC8406AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Trial #</t>
   </si>
@@ -123,12 +123,24 @@
 * n2 = 8</t>
   </si>
   <si>
-    <t>validation_split=0.25</t>
-  </si>
-  <si>
     <t>* 3-Layer NN
 * n1 = 10
 * n2 = 10</t>
+  </si>
+  <si>
+    <t>Increased the second hidden layer to 8 nodes. Overall accuracy went up in training and testing</t>
+  </si>
+  <si>
+    <t>Decreased the learning rate by an order of magnitude and it had terrible consequences</t>
+  </si>
+  <si>
+    <t>Doubled the batch size and returned the learning rate back. The increase in batch size had no good affect</t>
+  </si>
+  <si>
+    <t>Set validation_split=0.25 and got a good bumb in training and test accuracy</t>
+  </si>
+  <si>
+    <t>Increased the number of nodes in the two hidden layers to 10 and it got me over the line</t>
   </si>
 </sst>
 </file>
@@ -249,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -282,9 +294,6 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -302,6 +311,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECD881C-90B5-3E4A-8289-E7A06430E593}">
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -666,47 +681,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="45.95" customHeight="1">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
     </row>
     <row r="2" spans="2:17" ht="30.95" customHeight="1">
       <c r="B2" s="4"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="17" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="2:17" ht="47.1" customHeight="1">
@@ -755,7 +770,7 @@
       <c r="P3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -802,12 +817,12 @@
       <c r="O4" s="10">
         <v>0.36959999999999998</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="12">
         <v>0.83799999999999997</v>
       </c>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="2:17" ht="50.25" customHeight="1">
+      <c r="Q4" s="19"/>
+    </row>
+    <row r="5" spans="2:17" ht="63.75" customHeight="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -850,12 +865,14 @@
       <c r="O5" s="10">
         <v>0.35020000000000001</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="12">
         <v>0.85399999999999998</v>
       </c>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="2:17" ht="56.25" customHeight="1">
+      <c r="Q5" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="57">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -898,12 +915,14 @@
       <c r="O6" s="10">
         <v>0.59179999999999999</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="12">
         <v>0.66400000000000003</v>
       </c>
-      <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="2:17" ht="49.5" customHeight="1">
+      <c r="Q6" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="71.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -946,12 +965,14 @@
       <c r="O7" s="10">
         <v>0.3856</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="12">
         <v>0.83</v>
       </c>
-      <c r="Q7" s="9"/>
-    </row>
-    <row r="8" spans="2:17" ht="42.75">
+      <c r="Q7" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="52.5" customHeight="1">
       <c r="B8" s="5">
         <v>4</v>
       </c>
@@ -994,19 +1015,19 @@
       <c r="O8" s="10">
         <v>0.28410000000000002</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>0.87</v>
       </c>
-      <c r="Q8" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="42.75">
+      <c r="Q8" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="57">
       <c r="B9" s="5">
         <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
@@ -1044,10 +1065,12 @@
       <c r="O9" s="10">
         <v>0.23230000000000001</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="12">
         <v>0.90400000000000003</v>
       </c>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="2:17" ht="24.95" customHeight="1">
       <c r="B10" s="5"/>

</xml_diff>